<commit_message>
Ban update Sieu cap vjp pr0
</commit_message>
<xml_diff>
--- a/src/main/java/time/Time.xlsx
+++ b/src/main/java/time/Time.xlsx
@@ -718,7 +718,9 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="n">
+        <v>3803.0</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -727,9 +729,15 @@
       <c r="H6" s="1">
         <v>3</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="I6" s="1" t="n">
+        <v>3839.0</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>2288.0</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>1405.0</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>

</xml_diff>